<commit_message>
Common: Added cotton stuff
</commit_message>
<xml_diff>
--- a/fixtures/cottons.xlsx
+++ b/fixtures/cottons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750733CD-0333-4BB4-AFF1-FBF4932E3EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC42C9A-4462-485B-B17E-EDF40EC428E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1530" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27060" yWindow="1725" windowWidth="23610" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <t>services</t>
   </si>
   <si>
-    <t>PuffSmith\Cotton\Import\CottonImport</t>
-  </si>
-  <si>
     <t>cottons</t>
   </si>
   <si>
@@ -46,9 +43,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>Super Sorb</t>
   </si>
   <si>
@@ -113,6 +107,12 @@
   </si>
   <si>
     <t>Exvape</t>
+  </si>
+  <si>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>cost</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +473,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -489,129 +489,167 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
-        <v>26</v>
+      <c r="C13">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>